<commit_message>
order changed V+ and V-
</commit_message>
<xml_diff>
--- a/table_1.xlsx
+++ b/table_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\E619545\OneDrive - UCB\Desktop\misc\Harmony\tnd-vaccine-effectiveness\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{22416C25-3BEC-4ECC-8D7B-CA2F8AF4542D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{58D9DCE9-DE09-422C-BCD5-EFD671B491F7}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{22416C25-3BEC-4ECC-8D7B-CA2F8AF4542D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A163423E-F3BB-4F16-B7B3-B0A28166EE66}"/>
   <bookViews>
-    <workbookView xWindow="910" yWindow="50" windowWidth="14400" windowHeight="7460" xr2:uid="{481E74A2-2C49-4CE8-8184-A11CCA12FEB2}"/>
+    <workbookView xWindow="1250" yWindow="390" windowWidth="7640" windowHeight="5230" xr2:uid="{481E74A2-2C49-4CE8-8184-A11CCA12FEB2}"/>
   </bookViews>
   <sheets>
     <sheet name="table 1" sheetId="1" r:id="rId1"/>
@@ -411,17 +411,17 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -453,21 +453,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D481AB3385833947B072A50C8F406807" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="deb48eaf7e49b18101954f469f0de25c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c6b1c3da-0fb1-4d94-92b5-cd562b6eeacb" xmlns:ns4="922eacfc-8696-4508-a3c9-5b18580b28d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="42a646bf7d9215bd6939175b8228d635" ns3:_="" ns4:_="">
     <xsd:import namespace="c6b1c3da-0fb1-4d94-92b5-cd562b6eeacb"/>
@@ -690,24 +675,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{176B9131-32AF-470D-9E78-4FE881BEE866}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F957FB5E-BE42-4382-BD79-A2F43273DA18}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F6D8356-391D-458C-AFBC-B2E30675FB3F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -724,4 +707,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F957FB5E-BE42-4382-BD79-A2F43273DA18}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{176B9131-32AF-470D-9E78-4FE881BEE866}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>